<commit_message>
Pipeline connected to UI
</commit_message>
<xml_diff>
--- a/excelwriter.xlsx
+++ b/excelwriter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{39F20FCE-C964-4EC6-8C7F-0D2D717B9B99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{82719923-D416-4A9B-A5DD-49A721A9B7E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,7 +515,7 @@
   <dimension ref="A1:X51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="X14" sqref="C2:X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>